<commit_message>
completed video 45 - working version of data provider code used to run testNG tests
</commit_message>
<xml_diff>
--- a/excelDriven.xlsx
+++ b/excelDriven.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
-    <t>Greeeting</t>
+    <t>Greeting</t>
   </si>
   <si>
     <t>Communication</t>
@@ -53,11 +53,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -316,35 +316,35 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>1.0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>143.0</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -352,13 +352,13 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>453.0</v>
       </c>
       <c r="D4" s="3" t="s">

</xml_diff>